<commit_message>
rerun benchmarks after removing irrelevant test
</commit_message>
<xml_diff>
--- a/sheets/ubuntu-chrome-all.xlsx
+++ b/sheets/ubuntu-chrome-all.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">pw-32</t>
   </si>
   <si>
-    <t xml:space="preserve">pw-45</t>
+    <t xml:space="preserve">pw-40</t>
   </si>
 </sst>
 </file>
@@ -307,7 +307,7 @@
                   <c:v>pw-32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>pw-45</c:v>
+                  <c:v>pw-40</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -319,40 +319,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.9</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.9</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.8</c:v>
+                  <c:v>24.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.7</c:v>
+                  <c:v>15.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.9</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.2</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,7 +445,7 @@
                   <c:v>pw-32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>pw-45</c:v>
+                  <c:v>pw-40</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -457,10 +457,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>6.9</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.8</c:v>
+                  <c:v>42.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.7</c:v>
@@ -469,10 +469,10 @@
                   <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.8</c:v>
+                  <c:v>15.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.2</c:v>
+                  <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.9</c:v>
@@ -481,16 +481,16 @@
                   <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.1</c:v>
+                  <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>16.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -583,7 +583,7 @@
                   <c:v>pw-32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>pw-45</c:v>
+                  <c:v>pw-40</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -595,16 +595,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.9</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.9</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.8</c:v>
+                  <c:v>24.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.2</c:v>
+                  <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15.8</c:v>
@@ -613,22 +613,22 @@
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.1</c:v>
+                  <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.7</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.1</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,11 +636,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="58329296"/>
-        <c:axId val="53023300"/>
+        <c:axId val="2234320"/>
+        <c:axId val="33178210"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58329296"/>
+        <c:axId val="2234320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +668,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53023300"/>
+        <c:crossAx val="33178210"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -676,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53023300"/>
+        <c:axId val="33178210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +713,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58329296"/>
+        <c:crossAx val="2234320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -765,16 +765,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>287640</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>741600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -782,8 +782,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4775760" y="1577880"/>
-        <a:ext cx="5764320" cy="3241440"/>
+        <a:off x="6486120" y="1185840"/>
+        <a:ext cx="5764680" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -910,7 +910,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -967,40 +967,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>42.9</v>
+        <v>42.7</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>24.8</v>
+        <v>24.6</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>17</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>15.7</v>
+        <v>15.8</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>10.2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>9.8</v>
+        <v>10</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>10.2</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>11</v>
+        <v>10.9</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>14.9</v>
+        <v>14.8</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>18.2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,10 +1008,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>6.9</v>
+        <v>7.8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>42.8</v>
+        <v>42.6</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>24.7</v>
@@ -1020,10 +1020,10 @@
         <v>17.1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>10.2</v>
+        <v>10.3</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>9.9</v>
@@ -1032,16 +1032,16 @@
         <v>9.9</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>10.1</v>
+        <v>10.2</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>10.8</v>
+        <v>11</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>14.8</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>18</v>
+        <v>16.9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,16 +1049,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>7.9</v>
+        <v>6.8</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>42.9</v>
+        <v>42.7</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>24.8</v>
+        <v>24.7</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>17.2</v>
+        <v>17.1</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>15.8</v>
@@ -1067,22 +1067,22 @@
         <v>10.2</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>9.9</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>10.1</v>
+        <v>10.2</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>10.9</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>14.7</v>
+        <v>14.9</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>18.1</v>
+        <v>17.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun all tests after adding new context for each page
</commit_message>
<xml_diff>
--- a/sheets/ubuntu-chrome-all.xlsx
+++ b/sheets/ubuntu-chrome-all.xlsx
@@ -319,16 +319,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.8</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.7</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.6</c:v>
+                  <c:v>24.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15.8</c:v>
@@ -337,7 +337,7 @@
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>10</c:v>
@@ -346,13 +346,13 @@
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.8</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17</c:v>
+                  <c:v>16.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,19 +457,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.8</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.6</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.7</c:v>
+                  <c:v>24.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.9</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.3</c:v>
@@ -478,7 +478,7 @@
                   <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.2</c:v>
@@ -490,7 +490,7 @@
                   <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.9</c:v>
+                  <c:v>16.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,25 +595,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>6.8</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.7</c:v>
+                  <c:v>24.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.8</c:v>
+                  <c:v>15.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.9</c:v>
@@ -625,10 +625,10 @@
                   <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.2</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,11 +636,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2234320"/>
-        <c:axId val="33178210"/>
+        <c:axId val="31872452"/>
+        <c:axId val="53462575"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2234320"/>
+        <c:axId val="31872452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +668,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33178210"/>
+        <c:crossAx val="53462575"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -676,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33178210"/>
+        <c:axId val="53462575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +713,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2234320"/>
+        <c:crossAx val="31872452"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -766,15 +766,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>666360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:colOff>607320</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:colOff>682200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -782,8 +782,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6486120" y="1185840"/>
-        <a:ext cx="5764680" cy="3241440"/>
+        <a:off x="6427080" y="1099800"/>
+        <a:ext cx="5764320" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -910,7 +910,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -967,16 +967,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>7.8</v>
+        <v>6.9</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>42.7</v>
+        <v>42.8</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>24.6</v>
+        <v>24.8</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>17</v>
+        <v>17.1</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>15.8</v>
@@ -985,7 +985,7 @@
         <v>10.2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>10</v>
@@ -994,13 +994,13 @@
         <v>10.2</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>10.9</v>
+        <v>11</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>14.8</v>
+        <v>14.5</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>17</v>
+        <v>16.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,19 +1008,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>7.8</v>
+        <v>6.8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>42.6</v>
+        <v>42.8</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>24.7</v>
+        <v>24.8</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>17.1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>15.9</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>10.3</v>
@@ -1029,7 +1029,7 @@
         <v>9.9</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>10.2</v>
@@ -1041,7 +1041,7 @@
         <v>14.8</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>16.9</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,25 +1049,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>6.8</v>
+        <v>6.9</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>42.7</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>24.7</v>
+        <v>24.8</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>17.1</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>10.2</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>9.9</v>
@@ -1079,10 +1079,10 @@
         <v>10.9</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>14.9</v>
+        <v>15</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>17.2</v>
+        <v>16.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>